<commit_message>
geektime DSAA training week 04 assignment
</commit_message>
<xml_diff>
--- a/五毒表.xlsx
+++ b/五毒表.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$61</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="133">
   <si>
     <t>更新日期</t>
   </si>
@@ -257,6 +257,12 @@
     <t>O(lgn)</t>
   </si>
   <si>
+    <t>33. 搜索旋转排序数组</t>
+  </si>
+  <si>
+    <t>注意二分变形条件，先判断左右有序性</t>
+  </si>
+  <si>
     <t>回溯</t>
   </si>
   <si>
@@ -284,6 +290,9 @@
     <t>64. 最小路径和</t>
   </si>
   <si>
+    <t>总结dp的思路</t>
+  </si>
+  <si>
     <t>91. 解码方法</t>
   </si>
   <si>
@@ -294,6 +303,93 @@
   </si>
   <si>
     <t>72. 编辑距离</t>
+  </si>
+  <si>
+    <t>70. 爬楼梯</t>
+  </si>
+  <si>
+    <t>简单dfs</t>
+  </si>
+  <si>
+    <t>322. 零钱兑换</t>
+  </si>
+  <si>
+    <t>O(n2)</t>
+  </si>
+  <si>
+    <t>1143. 最长公共子序列</t>
+  </si>
+  <si>
+    <t>总结dp的思路 矩阵化</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>130. 被围绕的区域</t>
+  </si>
+  <si>
+    <t>dfs法</t>
+  </si>
+  <si>
+    <t>200. 岛屿数量</t>
+  </si>
+  <si>
+    <t>547. 省份数量</t>
+  </si>
+  <si>
+    <t>dfs法，注意visited的运用</t>
+  </si>
+  <si>
+    <t>463. 岛屿的周长</t>
+  </si>
+  <si>
+    <t>dfs法，注意周长关系的运用</t>
+  </si>
+  <si>
+    <t>695. 岛屿的最大面积</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>127. 单词接龙</t>
+  </si>
+  <si>
+    <t>？</t>
+  </si>
+  <si>
+    <t>trie</t>
+  </si>
+  <si>
+    <t>208. 实现 Trie (前缀树)</t>
+  </si>
+  <si>
+    <t>map实现，可以待换为数组</t>
+  </si>
+  <si>
+    <t>O(k)单词长度</t>
+  </si>
+  <si>
+    <t>O(n)单词数量</t>
+  </si>
+  <si>
+    <t>位运算</t>
+  </si>
+  <si>
+    <t>190. 颠倒二进制位</t>
+  </si>
+  <si>
+    <t>常规位运算</t>
+  </si>
+  <si>
+    <t>231. 2的幂</t>
+  </si>
+  <si>
+    <t>n&amp;(n-1)的运用</t>
+  </si>
+  <si>
+    <t>191. 位1的个数</t>
   </si>
   <si>
     <t>未知</t>
@@ -381,12 +477,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,24 +511,29 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color rgb="FF262626"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,17 +547,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -468,62 +561,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,8 +584,55 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,6 +644,22 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -586,7 +688,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,37 +730,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,31 +844,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,103 +868,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,13 +888,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,24 +962,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -859,30 +985,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -891,10 +993,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -903,137 +1005,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1052,9 +1154,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1091,61 +1190,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1496,32 +1589,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9" style="7"/>
-    <col min="2" max="2" width="20.9090909090909" style="8" customWidth="1"/>
-    <col min="3" max="3" width="5.81818181818182" style="8" customWidth="1"/>
-    <col min="4" max="4" width="33.2727272727273" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.72727272727273" style="8" customWidth="1"/>
-    <col min="6" max="6" width="7.54545454545455" style="7" customWidth="1"/>
-    <col min="7" max="7" width="5.54545454545455" style="7" customWidth="1"/>
-    <col min="8" max="10" width="10.6363636363636" style="7"/>
-    <col min="11" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="9" style="6"/>
+    <col min="2" max="2" width="20.9090909090909" style="7" customWidth="1"/>
+    <col min="3" max="3" width="5.81818181818182" style="7" customWidth="1"/>
+    <col min="4" max="4" width="36.6363636363636" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.72727272727273" style="7" customWidth="1"/>
+    <col min="6" max="6" width="7.54545454545455" style="6" customWidth="1"/>
+    <col min="7" max="7" width="5.54545454545455" style="6" customWidth="1"/>
+    <col min="8" max="10" width="10.6363636363636" style="6"/>
+    <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="8">
         <v>44276</v>
       </c>
     </row>
@@ -1529,16 +1622,16 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1564,285 +1657,285 @@
       </c>
     </row>
     <row r="3" ht="28" spans="1:10">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="12">
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="11">
         <v>44241</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>44256</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>44265</v>
       </c>
     </row>
     <row r="4" ht="28" spans="2:8">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="11">
         <v>44241</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="2:5">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" s="2" customFormat="1" ht="17" spans="2:5">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>44241</v>
       </c>
     </row>
     <row r="8" ht="28" spans="2:8">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="11">
         <v>44264</v>
       </c>
     </row>
     <row r="9" ht="17" spans="2:8">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>1</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>44272</v>
       </c>
     </row>
     <row r="10" ht="17" spans="2:8">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>1</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="11">
         <v>44274</v>
       </c>
     </row>
     <row r="11" ht="17" spans="2:9">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="G11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="11">
         <v>44247</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="12" ht="28" spans="1:8">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>1</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="G12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="11">
         <v>44267</v>
       </c>
     </row>
     <row r="13" ht="30.5" spans="2:9">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="H13" s="12">
+      <c r="F13" s="15"/>
+      <c r="H13" s="11">
         <v>44251</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="32">
         <v>44279</v>
       </c>
     </row>
     <row r="14" ht="28" spans="1:9">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>1</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="12">
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="11">
         <v>44246</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>44269</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" ht="30.5" spans="2:8">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="19">
         <v>0</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="21">
         <v>44272</v>
       </c>
     </row>
@@ -1850,405 +1943,411 @@
       <c r="A16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="23">
         <v>0</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="12">
+      <c r="G16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="11">
         <v>44272</v>
       </c>
     </row>
-    <row r="17" ht="17" spans="1:8">
-      <c r="A17" s="7" t="s">
+    <row r="17" ht="17" spans="1:9">
+      <c r="A17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>1</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="12">
+      <c r="G17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="11">
         <v>44268</v>
       </c>
+      <c r="I17" s="31">
+        <v>44287</v>
+      </c>
     </row>
     <row r="18" ht="17" spans="2:8">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>1</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="12">
+      <c r="G18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="11">
         <v>44268</v>
       </c>
     </row>
     <row r="19" ht="17" spans="2:8">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="12">
+      <c r="G19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="11">
         <v>44268</v>
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="12">
+      <c r="G20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="11">
         <v>44268</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="32">
         <v>44277</v>
       </c>
     </row>
     <row r="21" ht="28" spans="2:8">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="12">
+      <c r="G21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="11">
         <v>44268</v>
       </c>
     </row>
     <row r="22" ht="17" spans="2:8">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>1</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="12">
+      <c r="G22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="23" ht="17" spans="2:8">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>1</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="12">
+      <c r="G23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="24" ht="17" spans="2:8">
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>1</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="12">
+      <c r="G24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="25" customFormat="1" ht="30.5" spans="1:8">
-      <c r="A25" s="7"/>
-      <c r="B25" s="18" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <v>0</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="12">
+      <c r="F25" s="15"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" ht="30.5" spans="2:9">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="19">
         <v>0</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="H26" s="23">
+      <c r="F26" s="20"/>
+      <c r="H26" s="21">
         <v>44275</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="32">
         <v>44280</v>
       </c>
     </row>
     <row r="27" s="5" customFormat="1" ht="17" spans="1:5">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" s="5" customFormat="1" ht="17" spans="2:5">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-    </row>
-    <row r="29" s="6" customFormat="1" ht="17" spans="2:8">
-      <c r="B29" s="30" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+    </row>
+    <row r="29" s="4" customFormat="1" ht="17" spans="2:8">
+      <c r="B29" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="H29" s="33">
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="H29" s="29">
         <v>44278</v>
       </c>
     </row>
-    <row r="30" s="3" customFormat="1" ht="28" spans="1:8">
+    <row r="30" s="3" customFormat="1" ht="28" spans="1:9">
       <c r="A30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="21"/>
-      <c r="H30" s="23">
+      <c r="E30" s="19"/>
+      <c r="H30" s="21">
         <v>44271</v>
+      </c>
+      <c r="I30" s="31">
+        <v>44289</v>
       </c>
     </row>
     <row r="31" s="4" customFormat="1" ht="17" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <v>1</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="12">
+      <c r="G31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="32" s="4" customFormat="1" ht="34" spans="2:8">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <v>1</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="12">
+      <c r="G32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="33" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <v>1</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="12">
+      <c r="G33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="11">
         <v>44275</v>
       </c>
     </row>
     <row r="34" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <v>0</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="12">
+      <c r="G34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="11">
         <v>44275</v>
       </c>
     </row>
@@ -2256,240 +2355,591 @@
       <c r="A35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>1</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="12">
+      <c r="G35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="11">
         <v>44275</v>
       </c>
     </row>
-    <row r="36" s="4" customFormat="1" ht="17" spans="1:8">
-      <c r="A36" s="4" t="s">
+    <row r="36" s="4" customFormat="1" ht="17" spans="2:8">
+      <c r="B36" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="C36" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="12">
-        <v>44276</v>
+      <c r="E36" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="31">
+        <v>44289</v>
       </c>
     </row>
     <row r="37" s="4" customFormat="1" ht="17" spans="1:8">
       <c r="A37" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="C37" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="E37" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="11">
+        <v>44276</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="1" ht="17" spans="1:8">
+      <c r="A38" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="35">
+      <c r="D38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="32">
         <v>44281</v>
       </c>
     </row>
-    <row r="38" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B38" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="34" t="s">
+    <row r="39" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B39" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="35">
+      <c r="D39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="32">
         <v>44281</v>
       </c>
-    </row>
-    <row r="39" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B39" s="19" t="s">
+      <c r="I39" s="31">
+        <v>44286</v>
+      </c>
+    </row>
+    <row r="40" s="4" customFormat="1" ht="17" spans="2:8">
+      <c r="B40" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="E40" s="7"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="32">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="41" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B41" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="35">
+      <c r="D41" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="32">
         <v>44281</v>
       </c>
-    </row>
-    <row r="40" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B40" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="34" t="s">
+      <c r="I41" s="31">
+        <v>44285</v>
+      </c>
+    </row>
+    <row r="42" s="4" customFormat="1" ht="17" spans="2:8">
+      <c r="B42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="35">
-        <v>44281</v>
-      </c>
-    </row>
-    <row r="41" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B41" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="34" t="s">
+      <c r="E42" s="7"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="32">
+        <v>44283</v>
+      </c>
+    </row>
+    <row r="43" s="4" customFormat="1" ht="17" spans="2:8">
+      <c r="B43" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D43" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="32">
+        <v>44283</v>
+      </c>
+    </row>
+    <row r="44" s="4" customFormat="1" ht="17" spans="2:8">
+      <c r="B44" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="35">
+      <c r="E44" s="7"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="32">
         <v>44283</v>
       </c>
     </row>
-    <row r="42" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B42" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="34" t="s">
+    <row r="45" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B45" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="31">
+        <v>44258</v>
+      </c>
+      <c r="I45" s="31">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="46" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B46" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D46" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="35">
-        <v>44283</v>
-      </c>
-    </row>
-    <row r="43" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B43" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="34" t="s">
+      <c r="E46" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="31">
+        <v>44285</v>
+      </c>
+      <c r="I46" s="32"/>
+    </row>
+    <row r="47" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B47" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="31">
+        <v>44284</v>
+      </c>
+      <c r="I47" s="32"/>
+    </row>
+    <row r="48" s="4" customFormat="1" ht="17" spans="1:8">
+      <c r="A48" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="31">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="49" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B49" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="31">
+        <v>44288</v>
+      </c>
+      <c r="I49" s="31">
+        <v>44289</v>
+      </c>
+    </row>
+    <row r="50" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B50" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I50" s="32"/>
+    </row>
+    <row r="51" s="4" customFormat="1" ht="17.5" spans="2:9">
+      <c r="B51" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I51" s="32"/>
+    </row>
+    <row r="52" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B52" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I52" s="32"/>
+    </row>
+    <row r="53" s="4" customFormat="1" ht="17" spans="1:9">
+      <c r="A53" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="35">
-        <v>44283</v>
-      </c>
-    </row>
-    <row r="44" s="4" customFormat="1" ht="17" spans="2:8">
-      <c r="B44" s="19"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="12"/>
-    </row>
-    <row r="45" s="2" customFormat="1" ht="17" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="14" t="s">
+      <c r="D53" s="7"/>
+      <c r="E53" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H53" s="31">
+        <v>44286</v>
+      </c>
+      <c r="I53" s="32"/>
+    </row>
+    <row r="54" s="4" customFormat="1" ht="17" spans="1:9">
+      <c r="A54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" s="2" customFormat="1" spans="2:5">
-      <c r="B46" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="13" t="s">
+      <c r="D54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="7">
+        <v>1</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H54" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I54" s="32"/>
+    </row>
+    <row r="55" s="4" customFormat="1" ht="17" spans="1:9">
+      <c r="A55" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="7">
+        <v>1</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I55" s="32"/>
+    </row>
+    <row r="56" s="4" customFormat="1" ht="17" spans="2:9">
+      <c r="B56" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I56" s="32"/>
+    </row>
+    <row r="57" s="4" customFormat="1" ht="17.5" spans="2:9">
+      <c r="B57" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="31">
+        <v>44289</v>
+      </c>
+      <c r="I57" s="32"/>
+    </row>
+    <row r="58" s="2" customFormat="1" ht="17" spans="1:5">
+      <c r="A58" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" s="2" customFormat="1" spans="2:5">
+      <c r="B59" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" s="2" customFormat="1" ht="17" spans="2:6">
-      <c r="B47" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="14" t="s">
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" s="2" customFormat="1" ht="17" spans="2:6">
+      <c r="B60" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="36"/>
-    </row>
-    <row r="48" ht="17" spans="2:8">
-      <c r="B48" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="34" t="s">
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="34"/>
+    </row>
+    <row r="61" ht="17" spans="2:8">
+      <c r="B61" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="25">
+      <c r="D61" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" s="23">
         <v>1</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="37">
+      <c r="F61" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="29">
         <v>44274</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E48">
+  <autoFilter ref="E1:E61">
     <extLst/>
   </autoFilter>
   <hyperlinks>
@@ -2500,13 +2950,13 @@
     <hyperlink ref="B18" r:id="rId5" display="590. N 叉树的后序遍历" tooltip="https://leetcode-cn.com/problems/n-ary-tree-postorder-traversal/"/>
     <hyperlink ref="B17" r:id="rId6" display="589. N 叉树的前序遍历" tooltip="https://leetcode-cn.com/problems/n-ary-tree-preorder-traversal/"/>
     <hyperlink ref="B28" r:id="rId7" display="49. 字母异位词分组" tooltip="https://leetcode-cn.com/problems/group-anagrams/"/>
-    <hyperlink ref="B45" r:id="rId8" display="264. 丑数 II" tooltip="https://leetcode-cn.com/problems/ugly-number-ii/"/>
+    <hyperlink ref="B58" r:id="rId8" display="264. 丑数 II" tooltip="https://leetcode-cn.com/problems/ugly-number-ii/"/>
     <hyperlink ref="B30" r:id="rId9" display="22. 括号生成" tooltip="https://leetcode-cn.com/problems/generate-parentheses/"/>
     <hyperlink ref="B9" r:id="rId10" display="350. 两个数组的交集 II" tooltip="https://leetcode-cn.com/problems/intersection-of-two-arrays-ii/"/>
     <hyperlink ref="B15" r:id="rId11" display="剑指 Offer 59 - I. 滑动窗口的最大值" tooltip="https://leetcode-cn.com/problems/hua-dong-chuang-kou-de-zui-da-zhi-lcof/"/>
     <hyperlink ref="B16" r:id="rId12" display="1021. 删除最外层的括号" tooltip="https://leetcode-cn.com/problems/remove-outermost-parentheses/"/>
     <hyperlink ref="B10" r:id="rId13" display="412. Fizz Buzz" tooltip="https://leetcode-cn.com/problems/fizz-buzz/"/>
-    <hyperlink ref="B48" r:id="rId14" display="258. 各位相加" tooltip="https://leetcode-cn.com/problems/add-digits/"/>
+    <hyperlink ref="B61" r:id="rId14" display="258. 各位相加" tooltip="https://leetcode-cn.com/problems/add-digits/"/>
     <hyperlink ref="B22" r:id="rId15" display="104. 二叉树的最大深度" tooltip="https://leetcode-cn.com/problems/maximum-depth-of-binary-tree/"/>
     <hyperlink ref="B23" r:id="rId16" display="111. 二叉树的最小深度" tooltip="https://leetcode-cn.com/problems/minimum-depth-of-binary-tree/"/>
     <hyperlink ref="B24" r:id="rId17" display="98. 验证二叉搜索树" tooltip="https://leetcode-cn.com/problems/validate-binary-search-tree/"/>
@@ -2518,16 +2968,30 @@
     <hyperlink ref="B34" r:id="rId23" display="874. 模拟行走机器人" tooltip="https://leetcode-cn.com/problems/walking-robot-simulation/"/>
     <hyperlink ref="B25" r:id="rId24" display="105. 从前序与中序遍历序列构造二叉树" tooltip="https://leetcode-cn.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/"/>
     <hyperlink ref="B35" r:id="rId25" display="50. Pow(x, n)" tooltip="https://leetcode-cn.com/problems/powx-n/"/>
-    <hyperlink ref="B36" r:id="rId26" display="51. N 皇后" tooltip="https://leetcode-cn.com/problems/n-queens/"/>
+    <hyperlink ref="B37" r:id="rId26" display="51. N 皇后" tooltip="https://leetcode-cn.com/problems/n-queens/"/>
     <hyperlink ref="B29" r:id="rId27" display="剑指 Offer 05. 替换空格" tooltip="https://leetcode-cn.com/problems/ti-huan-kong-ge-lcof/"/>
     <hyperlink ref="B13" r:id="rId28" display="剑指 Offer 06. 从尾到头打印链表" tooltip="https://leetcode-cn.com/problems/cong-wei-dao-tou-da-yin-lian-biao-lcof/"/>
-    <hyperlink ref="B38" r:id="rId29" display="213. 打家劫舍 II" tooltip="https://leetcode-cn.com/problems/house-robber-ii/"/>
-    <hyperlink ref="B37" r:id="rId30" display="198. 打家劫舍" tooltip="https://leetcode-cn.com/problems/house-robber/"/>
-    <hyperlink ref="B39" r:id="rId31" display="337. 打家劫舍 III" tooltip="https://leetcode-cn.com/problems/house-robber-iii/"/>
-    <hyperlink ref="B40" r:id="rId32" display="64. 最小路径和" tooltip="https://leetcode-cn.com/problems/minimum-path-sum/"/>
-    <hyperlink ref="B41" r:id="rId33" display="91. 解码方法" tooltip="https://leetcode-cn.com/problems/decode-ways/"/>
-    <hyperlink ref="B42" r:id="rId34" display="221. 最大正方形" tooltip="https://leetcode-cn.com/problems/maximal-square/"/>
-    <hyperlink ref="B43" r:id="rId35" display="72. 编辑距离" tooltip="https://leetcode-cn.com/problems/edit-distance/"/>
+    <hyperlink ref="B39" r:id="rId29" display="213. 打家劫舍 II" tooltip="https://leetcode-cn.com/problems/house-robber-ii/"/>
+    <hyperlink ref="B38" r:id="rId30" display="198. 打家劫舍" tooltip="https://leetcode-cn.com/problems/house-robber/"/>
+    <hyperlink ref="B40" r:id="rId31" display="337. 打家劫舍 III" tooltip="https://leetcode-cn.com/problems/house-robber-iii/"/>
+    <hyperlink ref="B41" r:id="rId32" display="64. 最小路径和" tooltip="https://leetcode-cn.com/problems/minimum-path-sum/"/>
+    <hyperlink ref="B42" r:id="rId33" display="91. 解码方法" tooltip="https://leetcode-cn.com/problems/decode-ways/"/>
+    <hyperlink ref="B43" r:id="rId34" display="221. 最大正方形" tooltip="https://leetcode-cn.com/problems/maximal-square/"/>
+    <hyperlink ref="B44" r:id="rId35" display="72. 编辑距离" tooltip="https://leetcode-cn.com/problems/edit-distance/"/>
+    <hyperlink ref="B48" r:id="rId36" display="130. 被围绕的区域" tooltip="https://leetcode-cn.com/problems/surrounded-regions/"/>
+    <hyperlink ref="B54" r:id="rId37" display="208. 实现 Trie (前缀树)" tooltip="https://leetcode-cn.com/problems/implement-trie-prefix-tree/"/>
+    <hyperlink ref="B49" r:id="rId38" display="200. 岛屿数量" tooltip="https://leetcode-cn.com/problems/number-of-islands/"/>
+    <hyperlink ref="B55" r:id="rId39" display="190. 颠倒二进制位" tooltip="https://leetcode-cn.com/problems/reverse-bits/"/>
+    <hyperlink ref="B56" r:id="rId40" display="231. 2的幂" tooltip="https://leetcode-cn.com/problems/power-of-two/"/>
+    <hyperlink ref="B57" r:id="rId41" display="191. 位1的个数" tooltip="https://leetcode-cn.com/problems/number-of-1-bits/"/>
+    <hyperlink ref="B45" r:id="rId42" display="70. 爬楼梯" tooltip="https://leetcode-cn.com/problems/climbing-stairs/"/>
+    <hyperlink ref="B50" r:id="rId43" display="547. 省份数量" tooltip="https://leetcode-cn.com/problems/number-of-provinces/"/>
+    <hyperlink ref="B51" r:id="rId44" display="463. 岛屿的周长" tooltip="https://leetcode-cn.com/problems/island-perimeter/"/>
+    <hyperlink ref="B52" r:id="rId45" display="695. 岛屿的最大面积" tooltip="https://leetcode-cn.com/problems/max-area-of-island/"/>
+    <hyperlink ref="B53" r:id="rId46" display="127. 单词接龙" tooltip="https://leetcode-cn.com/problems/word-ladder/"/>
+    <hyperlink ref="B46" r:id="rId47" display="322. 零钱兑换" tooltip="https://leetcode-cn.com/problems/coin-change/"/>
+    <hyperlink ref="B47" r:id="rId48" display="1143. 最长公共子序列" tooltip="https://leetcode-cn.com/problems/longest-common-subsequence/"/>
+    <hyperlink ref="B36" r:id="rId49" display="33. 搜索旋转排序数组" tooltip="https://leetcode-cn.com/problems/search-in-rotated-sorted-array/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2555,44 +3019,44 @@
         <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>